<commit_message>
HOT-27 - Explain plans.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -22,289 +22,289 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="95">
   <si>
-    <t>High End</t>
-  </si>
-  <si>
-    <t>Middle Tier</t>
-  </si>
-  <si>
-    <t>Subpar</t>
-  </si>
-  <si>
-    <t>Lighweight Tier</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>DB2</t>
-  </si>
-  <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>SQL Server</t>
-  </si>
-  <si>
-    <t>MariaDB</t>
-  </si>
-  <si>
-    <t>MySQL</t>
-  </si>
-  <si>
-    <t>SAP ASE</t>
-  </si>
-  <si>
-    <t>Derby</t>
-  </si>
-  <si>
-    <t>HyperSQL</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>Catalog Term</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>database *2</t>
-  </si>
-  <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>CATALOG *2</t>
-  </si>
-  <si>
-    <t>catalog *2</t>
-  </si>
-  <si>
-    <t>Schema Term</t>
-  </si>
-  <si>
-    <t>schema</t>
-  </si>
-  <si>
-    <t>SCHEMA</t>
-  </si>
-  <si>
-    <t>Identifier default case</t>
-  </si>
-  <si>
-    <t>UPPER</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>Insensitive *3</t>
-  </si>
-  <si>
-    <t>Sensitive *4</t>
-  </si>
-  <si>
-    <t>Key Generation</t>
-  </si>
-  <si>
-    <t>Sequences</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Identities generated always</t>
-  </si>
-  <si>
-    <t>Since 12c</t>
-  </si>
-  <si>
-    <t>Identities generated by default</t>
-  </si>
-  <si>
-    <t>Identity columns per table</t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>multiple</t>
-  </si>
-  <si>
-    <t>Extra Features</t>
-  </si>
-  <si>
-    <t>Top-N rows</t>
-  </si>
-  <si>
-    <t>Query Pagination</t>
-  </si>
-  <si>
-    <t>Hierarchical Queries</t>
-  </si>
-  <si>
-    <t>Yes *7</t>
-  </si>
-  <si>
-    <t>Since 10.2.2</t>
-  </si>
-  <si>
-    <t>From 8.0</t>
-  </si>
-  <si>
-    <t>Yes *12</t>
-  </si>
-  <si>
-    <t>Virtual Columns</t>
-  </si>
-  <si>
-    <t>Yes *13</t>
-  </si>
-  <si>
-    <t>Yes *15</t>
-  </si>
-  <si>
-    <t>Yes *10</t>
-  </si>
-  <si>
-    <t>Since 5.7</t>
-  </si>
-  <si>
-    <t>Yes *18</t>
-  </si>
-  <si>
-    <t>Full Text Search</t>
-  </si>
-  <si>
-    <t>Index Optimization</t>
-  </si>
-  <si>
-    <t>Indexes on Expressions</t>
-  </si>
-  <si>
-    <t>Indexes on Expressions with UDF</t>
-  </si>
-  <si>
-    <t>Yes *16</t>
-  </si>
-  <si>
-    <t>Indexes on Virtual Columns</t>
-  </si>
-  <si>
-    <t>Yes *11</t>
-  </si>
-  <si>
-    <t>Yes *19</t>
-  </si>
-  <si>
-    <t>Optional indexes on FKs</t>
-  </si>
-  <si>
-    <t>Index Organized Tables (no heap)</t>
-  </si>
-  <si>
-    <t>Yes *9</t>
-  </si>
-  <si>
-    <t>Clustered Indexes (data in heap)</t>
-  </si>
-  <si>
-    <t>Yes *17</t>
-  </si>
-  <si>
-    <t>Non-key columns on Indexes</t>
-  </si>
-  <si>
-    <t>Yes *8</t>
-  </si>
-  <si>
-    <t>Partial Indexes</t>
-  </si>
-  <si>
-    <t>SQL Optimization</t>
-  </si>
-  <si>
-    <t>Explain Plan</t>
-  </si>
-  <si>
-    <t>Explain Plan without execution</t>
-  </si>
-  <si>
-    <t>Explain Plan with parameters</t>
-  </si>
-  <si>
-    <t>Yes *1</t>
-  </si>
-  <si>
-    <t>Yes *5</t>
-  </si>
-  <si>
-    <t>Yes *6</t>
-  </si>
-  <si>
-    <t>*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
-  </si>
-  <si>
-    <t>*2 Informed by the database, but not used internally.</t>
-  </si>
-  <si>
-    <t>*3 The identifier can be typed in any case. It will match other cases.</t>
-  </si>
-  <si>
-    <t>*4 The identifier will be stored in the case it was typed.</t>
-  </si>
-  <si>
-    <t>*5 Yes, but the parameter types must be specified (not the values).</t>
-  </si>
-  <si>
-    <t>*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
-  </si>
-  <si>
-    <t>*7 Not enabled by default. The DBA needs to enable them after installation.</t>
-  </si>
-  <si>
-    <t>*8 On unique indexes only.</t>
-  </si>
-  <si>
-    <t>*9 Only on InnoDB tables.</t>
-  </si>
-  <si>
-    <t>*10 Can use user-defined functions since 10.2.1</t>
-  </si>
-  <si>
-    <t>*11 Only persistent virtual columns can be indexed.</t>
-  </si>
-  <si>
-    <t>*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
-  </si>
-  <si>
-    <t>*13 Always persisted.</t>
-  </si>
-  <si>
-    <t>*14 User-defined functions are not allowed.</t>
-  </si>
-  <si>
-    <t>*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
-  </si>
-  <si>
-    <t>*16 Must use deterministic UDFs.</t>
-  </si>
-  <si>
-    <t>*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
-  </si>
-  <si>
-    <t>*18 Are always persistent columns.</t>
-  </si>
-  <si>
-    <t>*19 Only on materialized virtual columns.</t>
+    <t xml:space="preserve">High End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Tier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subpar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lighweight Tier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MariaDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HyperSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalog Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATALOG *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schema Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier default case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insensitive *3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitive *4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identities generated always</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 12c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identities generated by default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity columns per table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top-N rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Query Pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hierarchical Queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 10.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 8.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 5.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Text Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Expressions with UDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional indexes on FKs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Organized Tables (no heap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Indexes (data in heap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-key columns on Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan without execution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan with parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2 Informed by the database, but not used internally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*3 The identifier can be typed in any case. It will match other cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*4 The identifier will be stored in the case it was typed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*5 Yes, but the parameter types must be specified (not the values).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*7 Not enabled by default. The DBA needs to enable them after installation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*8 On unique indexes only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*9 Only on InnoDB tables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*10 Can use user-defined functions since 10.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*13 Always persisted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*14 User-defined functions are not allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*16 Must use deterministic UDFs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*18 Are always persistent columns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*19 Only on materialized virtual columns.</t>
   </si>
 </sst>
 </file>
@@ -312,7 +312,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -351,7 +351,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +386,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCCCC"/>
         <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
     <fill>
@@ -471,7 +477,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -572,15 +578,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,7 +590,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,7 +598,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -636,7 +638,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF66CC"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF000080"/>
@@ -684,21 +686,20 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5459183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,7 +1073,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -1107,7 +1108,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -1128,7 +1129,7 @@
       <c r="G13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="25" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="19" t="s">
@@ -1148,7 +1149,7 @@
       <c r="B14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="15" t="s">
@@ -1166,7 +1167,7 @@
       <c r="H14" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="27" t="s">
         <v>32</v>
       </c>
       <c r="J14" s="20" t="s">
@@ -1186,7 +1187,7 @@
       <c r="C15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="14" t="s">
@@ -1201,10 +1202,10 @@
       <c r="H15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="30" t="s">
+      <c r="I15" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K15" s="21" t="s">
@@ -1286,10 +1287,10 @@
       <c r="H18" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="30" t="s">
+      <c r="I18" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K18" s="24" t="s">
@@ -1321,10 +1322,10 @@
       <c r="H19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="30" t="s">
+      <c r="I19" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K19" s="24" t="s">
@@ -1356,10 +1357,10 @@
       <c r="H20" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I20" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="30" t="s">
+      <c r="I20" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K20" s="21" t="s">
@@ -1391,10 +1392,10 @@
       <c r="H21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="30" t="s">
+      <c r="I21" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K21" s="24" t="s">
@@ -1417,19 +1418,19 @@
       <c r="E22" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="26" t="s">
         <v>63</v>
       </c>
       <c r="H22" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="30" t="s">
+      <c r="I22" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K22" s="24" t="s">
@@ -1452,22 +1453,22 @@
       <c r="E23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="26" t="s">
         <v>63</v>
       </c>
       <c r="H23" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="31" t="s">
+      <c r="I23" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="30" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1478,7 +1479,7 @@
       <c r="B24" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="23" t="s">
@@ -1496,10 +1497,10 @@
       <c r="H24" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" s="30" t="s">
+      <c r="I24" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K24" s="24" t="s">
@@ -1531,10 +1532,10 @@
       <c r="H25" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J25" s="30" t="s">
+      <c r="I25" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K25" s="24" t="s">
@@ -1636,7 +1637,7 @@
       <c r="H28" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="I28" s="27" t="s">
         <v>32</v>
       </c>
       <c r="J28" s="20" t="s">
@@ -1656,22 +1657,22 @@
       <c r="C29" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="27" t="s">
+      <c r="G29" s="26" t="s">
         <v>75</v>
       </c>
       <c r="H29" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="27" t="s">
         <v>32</v>
       </c>
       <c r="J29" s="20" t="s">
@@ -1694,7 +1695,7 @@
       <c r="A32" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="K32" s="32"/>
+      <c r="K32" s="31"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">

</xml_diff>

<commit_message>
HOT-27 - Database features.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="101">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -223,21 +223,15 @@
     <t xml:space="preserve">Clustered Index Tables (IOTs, no heap)</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes *22</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yes *9</t>
   </si>
   <si>
-    <t xml:space="preserve">Clustered Tables (data in heap)</t>
+    <t xml:space="preserve">Clustering Indexes (separated)</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *21</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes *17</t>
-  </si>
-  <si>
     <t xml:space="preserve">Non-key columns on Indexes</t>
   </si>
   <si>
@@ -316,7 +310,7 @@
     <t xml:space="preserve">*16 Must use deterministic UDFs.</t>
   </si>
   <si>
-    <t xml:space="preserve">*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
+    <t xml:space="preserve">*17 (unused)</t>
   </si>
   <si>
     <t xml:space="preserve">*18 Are always persistent columns.</t>
@@ -329,9 +323,6 @@
   </si>
   <si>
     <t xml:space="preserve">*21 The database does not ensure, but tries to keep the rows in the cluster index order. Periodical maintenance is needed to ensure this ordering.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*22 SQL Server literature calls IOTs as “Clustered Tables” or “Clustered Index Tables”. However, these do NOT have a heap.</t>
   </si>
 </sst>
 </file>
@@ -694,24 +685,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,16 +1515,16 @@
         <v>33</v>
       </c>
       <c r="E24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="G24" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>33</v>
+        <v>67</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="I24" s="26" t="s">
         <v>33</v>
@@ -1548,16 +1539,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>70</v>
-      </c>
       <c r="D25" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>33</v>
@@ -1568,11 +1559,11 @@
       <c r="G25" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="31" t="s">
-        <v>71</v>
+      <c r="H25" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="J25" s="28" t="s">
         <v>33</v>
@@ -1584,13 +1575,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>33</v>
@@ -1620,7 +1611,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>32</v>
@@ -1656,7 +1647,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>6</v>
@@ -1692,7 +1683,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>32</v>
@@ -1728,7 +1719,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>32</v>
@@ -1764,25 +1755,25 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="29" t="s">
+      <c r="F31" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>81</v>
-      </c>
       <c r="G31" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H31" s="25" t="s">
         <v>33</v>
@@ -1804,116 +1795,111 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J34" s="32"/>
       <c r="K34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOT-27 - More database features.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="111">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">multiple</t>
   </si>
   <si>
-    <t xml:space="preserve">3. Important Features</t>
+    <t xml:space="preserve">3. Core Features</t>
   </si>
   <si>
     <t xml:space="preserve">Top-N rows</t>
@@ -151,7 +151,16 @@
     <t xml:space="preserve">Query Pagination</t>
   </si>
   <si>
-    <t xml:space="preserve">4. Extra Features</t>
+    <t xml:space="preserve">4. Advanced Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With clause supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
   </si>
   <si>
     <t xml:space="preserve">Hierarchical Queries</t>
@@ -169,6 +178,12 @@
     <t xml:space="preserve">Yes *12</t>
   </si>
   <si>
+    <t xml:space="preserve">Lateral supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grouping Sets supported</t>
+  </si>
+  <si>
     <t xml:space="preserve">Virtual Columns</t>
   </si>
   <si>
@@ -185,6 +200,21 @@
   </si>
   <si>
     <t xml:space="preserve">Yes *18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporal Tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row Pattern Maching supported</t>
   </si>
   <si>
     <t xml:space="preserve">Full Text Search</t>
@@ -475,7 +505,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -584,11 +614,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,24 +735,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,198 +1254,218 @@
       <c r="B15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>46</v>
-      </c>
       <c r="G15" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>32</v>
+        <v>45</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="L15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="G16" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="H16" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J16" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="30" t="s">
-        <v>33</v>
+      <c r="J16" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="L16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="20"/>
+        <v>52</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="30" t="s">
+        <v>46</v>
+      </c>
       <c r="L17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>15</v>
+      <c r="A18" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="L18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>33</v>
+      <c r="G19" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="H19" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="30" t="s">
+      <c r="I19" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="35" t="s">
         <v>33</v>
       </c>
       <c r="L19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I20" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J20" s="28" t="s">
-        <v>33</v>
+      <c r="E20" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>32</v>
@@ -1409,23 +1479,23 @@
       <c r="E21" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="24" t="s">
-        <v>61</v>
+      <c r="F21" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="L21" s="0"/>
     </row>
@@ -1436,38 +1506,38 @@
       <c r="B22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="28" t="s">
-        <v>33</v>
+      <c r="C22" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="K22" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>32</v>
@@ -1475,143 +1545,143 @@
       <c r="C23" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>33</v>
+      <c r="D23" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>33</v>
+      <c r="C24" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="K24" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" s="28" t="s">
-        <v>33</v>
+        <v>65</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J26" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="K26" s="30" t="s">
-        <v>33</v>
+      <c r="A26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="L26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>32</v>
@@ -1622,8 +1692,8 @@
       <c r="D27" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>32</v>
+      <c r="E27" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>33</v>
@@ -1631,59 +1701,59 @@
       <c r="G27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="25" t="s">
-        <v>33</v>
+      <c r="H27" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="I27" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J27" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="K27" s="30" t="s">
+      <c r="J27" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="35" t="s">
         <v>33</v>
       </c>
       <c r="L27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>15</v>
+      <c r="A28" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="L28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>32</v>
@@ -1697,11 +1767,11 @@
       <c r="E29" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>32</v>
+      <c r="F29" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>32</v>
@@ -1712,14 +1782,14 @@
       <c r="J29" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="23" t="s">
-        <v>32</v>
+      <c r="K29" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="L29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>32</v>
@@ -1727,179 +1797,467 @@
       <c r="C30" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>32</v>
+      <c r="D30" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>32</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>32</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="23" t="s">
-        <v>32</v>
+      <c r="J30" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="L30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="29" t="s">
+      <c r="B32" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="G32" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="B33" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="G31" s="27" t="s">
+      <c r="D33" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="H31" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J31" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="K31" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="L31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="E33" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J33" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J33" s="0"/>
-      <c r="K33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="B34" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
+      <c r="D34" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="13" t="s">
         <v>82</v>
       </c>
+      <c r="B35" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="7" t="s">
         <v>83</v>
       </c>
+      <c r="B36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="13" t="s">
         <v>84</v>
       </c>
+      <c r="B37" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K37" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="13" t="s">
         <v>85</v>
       </c>
+      <c r="B38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="B39" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>87</v>
-      </c>
+      <c r="J40" s="0"/>
+      <c r="K40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>88</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="J41" s="0"/>
+      <c r="K41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>89</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOT-27 - Basic plugin up. Half tested.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="112">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes *12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraint Deferrability supported</t>
   </si>
   <si>
     <t xml:space="preserve">Lateral supported</t>
@@ -505,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -614,22 +617,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -638,15 +625,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -735,24 +718,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,16 +1251,16 @@
       <c r="G15" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="30" t="s">
+      <c r="H15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="20" t="s">
         <v>46</v>
       </c>
       <c r="L15" s="0"/>
@@ -1290,7 +1272,7 @@
       <c r="B16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="17" t="s">
@@ -1311,7 +1293,7 @@
       <c r="I16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="28" t="s">
         <v>33</v>
       </c>
       <c r="K16" s="23" t="s">
@@ -1326,32 +1308,32 @@
       <c r="B17" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>32</v>
+      <c r="C17" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>46</v>
+      <c r="E17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="L17" s="0"/>
     </row>
@@ -1368,25 +1350,25 @@
       <c r="D18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K18" s="30" t="s">
+      <c r="E18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="20" t="s">
         <v>46</v>
       </c>
       <c r="L18" s="0"/>
@@ -1399,67 +1381,67 @@
         <v>32</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>56</v>
+        <v>32</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>33</v>
+      <c r="F19" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="L19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K20" s="30" t="s">
-        <v>46</v>
+      <c r="J20" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="L20" s="0"/>
     </row>
@@ -1467,34 +1449,34 @@
       <c r="A21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>32</v>
+      <c r="B21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K21" s="30" t="s">
+      <c r="E21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="20" t="s">
         <v>46</v>
       </c>
       <c r="L21" s="0"/>
@@ -1506,31 +1488,31 @@
       <c r="B22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="33" t="s">
-        <v>46</v>
+      <c r="C22" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" s="30" t="s">
+      <c r="E22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="20" t="s">
         <v>46</v>
       </c>
       <c r="L22" s="0"/>
@@ -1542,31 +1524,31 @@
       <c r="B23" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K23" s="30" t="s">
+      <c r="C23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23" s="20" t="s">
         <v>46</v>
       </c>
       <c r="L23" s="0"/>
@@ -1578,31 +1560,31 @@
       <c r="B24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K24" s="30" t="s">
+      <c r="C24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" s="20" t="s">
         <v>46</v>
       </c>
       <c r="L24" s="0"/>
@@ -1611,107 +1593,107 @@
       <c r="A25" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K25" s="30" t="s">
+      <c r="B25" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="20" t="s">
         <v>46</v>
       </c>
       <c r="L25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J27" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K27" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="L26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K27" s="35" t="s">
-        <v>33</v>
       </c>
       <c r="L27" s="0"/>
     </row>
@@ -1720,10 +1702,10 @@
         <v>68</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>32</v>
@@ -1743,118 +1725,118 @@
       <c r="I28" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K28" s="35" t="s">
+      <c r="J28" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="29" t="s">
         <v>33</v>
       </c>
       <c r="L28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>32</v>
+      <c r="C29" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>32</v>
+      <c r="E29" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I29" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K29" s="24" t="s">
-        <v>71</v>
+      <c r="I29" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="L29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>32</v>
+      <c r="G30" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="35" t="s">
-        <v>33</v>
+      <c r="J30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="L30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I31" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K31" s="35" t="s">
+      <c r="I31" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="29" t="s">
         <v>33</v>
       </c>
       <c r="L31" s="0"/>
@@ -1866,20 +1848,20 @@
       <c r="B32" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>33</v>
+      <c r="C32" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>77</v>
+      <c r="F32" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>32</v>
@@ -1887,65 +1869,65 @@
       <c r="I32" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K32" s="35" t="s">
+      <c r="J32" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="29" t="s">
         <v>33</v>
       </c>
       <c r="L32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H33" s="25" t="s">
-        <v>33</v>
+      <c r="G33" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="I33" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J33" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K33" s="35" t="s">
+      <c r="J33" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="29" t="s">
         <v>33</v>
       </c>
       <c r="L33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>32</v>
+      <c r="D34" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="F34" s="24" t="s">
         <v>33</v>
@@ -1959,26 +1941,26 @@
       <c r="I34" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J34" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K34" s="35" t="s">
+      <c r="J34" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="29" t="s">
         <v>33</v>
       </c>
       <c r="L34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>32</v>
+      <c r="D35" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>32</v>
@@ -1995,83 +1977,83 @@
       <c r="I35" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J35" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K35" s="35" t="s">
+      <c r="J35" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="29" t="s">
         <v>33</v>
       </c>
       <c r="L35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K36" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="L36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C37" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G37" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H37" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="10" t="s">
+      <c r="I37" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J36" s="11" t="s">
+      <c r="J37" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="K37" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="L36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I37" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J37" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K37" s="23" t="s">
-        <v>32</v>
       </c>
       <c r="L37" s="0"/>
     </row>
@@ -2103,8 +2085,8 @@
       <c r="I38" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="32" t="s">
-        <v>33</v>
+      <c r="J38" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="K38" s="23" t="s">
         <v>32</v>
@@ -2121,40 +2103,69 @@
       <c r="C39" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I39" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="B40" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="31" t="s">
+      <c r="E40" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G39" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K39" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="L39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="0"/>
-      <c r="K40" s="0"/>
+      <c r="F40" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J40" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="J41" s="0"/>
       <c r="K41" s="0"/>
     </row>
@@ -2162,13 +2173,15 @@
       <c r="A42" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J42" s="37"/>
-      <c r="K42" s="37"/>
+      <c r="J42" s="0"/>
+      <c r="K42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>92</v>
       </c>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -2258,6 +2271,11 @@
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOT-27 - Functional eclipse plugin - v-alpha1.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="124">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -148,9 +148,15 @@
     <t xml:space="preserve">Top-N rows</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Top-N Rows</t>
+  </si>
+  <si>
     <t xml:space="preserve">Query Pagination</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Query Pagination</t>
+  </si>
+  <si>
     <t xml:space="preserve">4. Advanced Features</t>
   </si>
   <si>
@@ -229,18 +235,27 @@
     <t xml:space="preserve">Indexes on Expressions</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Indexes on Expressions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indexes on Expressions with UDF</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *16</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Indexes on UDF Expressions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Descending Indexes</t>
   </si>
   <si>
     <t xml:space="preserve">No *20</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Descending Indexes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indexes on Virtual Columns</t>
   </si>
   <si>
@@ -250,34 +265,55 @@
     <t xml:space="preserve">Yes *19</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Indexes on Virtual Columns</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optional indexes on FKs</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - </t>
+  </si>
+  <si>
     <t xml:space="preserve">Clustered Index Tables (IOTs, no heap)</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *9</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Clustered Index Tables</t>
+  </si>
+  <si>
     <t xml:space="preserve">Clustering Indexes (separated)</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *21</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Clustering Index</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-key columns on Indexes</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *8</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Non-key Columns on Indexes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Partial Indexes</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;database&gt; - Partial Indexes</t>
+  </si>
+  <si>
     <t xml:space="preserve">6. SQL Optimization</t>
   </si>
   <si>
     <t xml:space="preserve">Explain Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Execution Plan</t>
   </si>
   <si>
     <t xml:space="preserve">Explain Plan without execution</t>
@@ -718,23 +754,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,10 +1193,13 @@
         <v>32</v>
       </c>
       <c r="L12" s="0"/>
+      <c r="M12" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>32</v>
@@ -1192,10 +1232,13 @@
         <v>32</v>
       </c>
       <c r="L13" s="0"/>
+      <c r="M13" s="0" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>6</v>
@@ -1231,7 +1274,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>32</v>
@@ -1246,34 +1289,34 @@
         <v>32</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>32</v>
@@ -1282,16 +1325,16 @@
         <v>32</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H16" s="25" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J16" s="28" t="s">
         <v>33</v>
@@ -1303,7 +1346,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>32</v>
@@ -1339,7 +1382,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>32</v>
@@ -1351,31 +1394,31 @@
         <v>32</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>32</v>
@@ -1390,52 +1433,52 @@
         <v>32</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J20" s="28" t="s">
         <v>33</v>
@@ -1447,43 +1490,43 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>32</v>
@@ -1498,64 +1541,64 @@
         <v>32</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>32</v>
@@ -1564,106 +1607,106 @@
         <v>32</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>6</v>
@@ -1699,7 +1742,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>32</v>
@@ -1732,13 +1775,16 @@
         <v>33</v>
       </c>
       <c r="L28" s="0"/>
+      <c r="M28" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>33</v>
@@ -1768,10 +1814,13 @@
         <v>33</v>
       </c>
       <c r="L29" s="0"/>
+      <c r="M29" s="0" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>32</v>
@@ -1786,10 +1835,10 @@
         <v>32</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H30" s="17" t="s">
         <v>32</v>
@@ -1801,13 +1850,16 @@
         <v>32</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L30" s="0"/>
+      <c r="M30" s="0" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>32</v>
@@ -1822,13 +1874,13 @@
         <v>32</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>32</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>32</v>
@@ -1840,10 +1892,13 @@
         <v>33</v>
       </c>
       <c r="L31" s="0"/>
+      <c r="M31" s="0" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>32</v>
@@ -1876,10 +1931,13 @@
         <v>33</v>
       </c>
       <c r="L32" s="0"/>
+      <c r="M32" s="0" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>32</v>
@@ -1894,10 +1952,10 @@
         <v>32</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>32</v>
@@ -1912,19 +1970,22 @@
         <v>33</v>
       </c>
       <c r="L33" s="0"/>
+      <c r="M33" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>33</v>
@@ -1948,16 +2009,19 @@
         <v>33</v>
       </c>
       <c r="L34" s="0"/>
+      <c r="M34" s="0" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>33</v>
@@ -1984,10 +2048,13 @@
         <v>33</v>
       </c>
       <c r="L35" s="0"/>
+      <c r="M35" s="0" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>32</v>
@@ -2020,10 +2087,13 @@
         <v>33</v>
       </c>
       <c r="L36" s="0"/>
+      <c r="M36" s="0" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>6</v>
@@ -2059,7 +2129,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>32</v>
@@ -2092,10 +2162,13 @@
         <v>32</v>
       </c>
       <c r="L38" s="0"/>
+      <c r="M38" s="0" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>32</v>
@@ -2131,7 +2204,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>32</v>
@@ -2140,16 +2213,16 @@
         <v>32</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="H40" s="25" t="s">
         <v>33</v>
@@ -2171,111 +2244,111 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="J42" s="0"/>
       <c r="K42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="J43" s="32"/>
       <c r="K43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOT27 - Documenting recursive joins.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -208,7 +208,7 @@
     <t>Yes *13</t>
   </si>
   <si>
-    <t>Yes *15</t>
+    <t>No *15</t>
   </si>
   <si>
     <t>Yes *10</t>
@@ -358,7 +358,7 @@
     <t>*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
   </si>
   <si>
-    <t>*7 Not enabled by default. The DBA needs to enable them after installation.</t>
+    <t>*7 Recursive CTEs work well. Old fashioned “connect by” queries are not enabled by default (after installation)</t>
   </si>
   <si>
     <t>*8 On unique indexes only.</t>
@@ -688,19 +688,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -795,22 +795,22 @@
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O24" activeCellId="0" sqref="O24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5459183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,7 +1356,7 @@
       <c r="B16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="19" t="s">
@@ -1377,7 +1377,7 @@
       <c r="I16" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="31" t="s">
         <v>34</v>
       </c>
       <c r="K16" s="25" t="s">
@@ -1413,10 +1413,10 @@
       <c r="I17" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="33" t="s">
+      <c r="J17" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L17" s="0"/>
@@ -1446,10 +1446,10 @@
       <c r="H18" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="31" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="25" t="s">
@@ -1539,7 +1539,7 @@
       <c r="C21" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="28" t="s">
         <v>62</v>
       </c>
       <c r="E21" s="17" t="s">
@@ -1557,10 +1557,10 @@
       <c r="I21" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="J21" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="33" t="s">
+      <c r="J21" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L21" s="0"/>
@@ -1845,10 +1845,10 @@
       <c r="I29" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J29" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="33" t="s">
+      <c r="J29" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L29" s="0"/>
@@ -1884,10 +1884,10 @@
       <c r="I30" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" s="33" t="s">
+      <c r="J30" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L30" s="0"/>
@@ -1962,10 +1962,10 @@
       <c r="I32" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" s="33" t="s">
+      <c r="J32" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L32" s="0"/>
@@ -2001,10 +2001,10 @@
       <c r="I33" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J33" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" s="33" t="s">
+      <c r="J33" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L33" s="0"/>
@@ -2040,10 +2040,10 @@
       <c r="I34" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J34" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" s="33" t="s">
+      <c r="J34" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L34" s="0"/>
@@ -2058,7 +2058,7 @@
       <c r="B35" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="34" t="s">
         <v>91</v>
       </c>
       <c r="D35" s="35" t="s">
@@ -2079,10 +2079,10 @@
       <c r="I35" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35" s="33" t="s">
+      <c r="J35" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L35" s="0"/>
@@ -2097,7 +2097,7 @@
       <c r="B36" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="34" t="s">
         <v>94</v>
       </c>
       <c r="D36" s="28" t="s">
@@ -2118,10 +2118,10 @@
       <c r="I36" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J36" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K36" s="33" t="s">
+      <c r="J36" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L36" s="0"/>
@@ -2157,10 +2157,10 @@
       <c r="I37" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J37" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K37" s="33" t="s">
+      <c r="J37" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="32" t="s">
         <v>34</v>
       </c>
       <c r="L37" s="0"/>
@@ -2271,7 +2271,7 @@
       <c r="I40" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="32" t="s">
+      <c r="J40" s="31" t="s">
         <v>34</v>
       </c>
       <c r="K40" s="25" t="s">
@@ -2289,16 +2289,16 @@
       <c r="C41" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="33" t="s">
         <v>103</v>
       </c>
       <c r="E41" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="G41" s="31" t="s">
+      <c r="G41" s="34" t="s">
         <v>105</v>
       </c>
       <c r="H41" s="28" t="s">
@@ -2307,7 +2307,7 @@
       <c r="I41" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J41" s="32" t="s">
+      <c r="J41" s="31" t="s">
         <v>34</v>
       </c>
       <c r="K41" s="25" t="s">

</xml_diff>

<commit_message>
HOT27 - Adding recursive query research.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,390 +20,384 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="128">
-  <si>
-    <t>Features \ League</t>
-  </si>
-  <si>
-    <t>High End</t>
-  </si>
-  <si>
-    <t>Superior</t>
-  </si>
-  <si>
-    <t>Middle Tier</t>
-  </si>
-  <si>
-    <t>Subpar</t>
-  </si>
-  <si>
-    <t>Lighweight Tier</t>
-  </si>
-  <si>
-    <t>1. Organization</t>
-  </si>
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>DB2</t>
-  </si>
-  <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>SQL Server</t>
-  </si>
-  <si>
-    <t>MariaDB</t>
-  </si>
-  <si>
-    <t>MySQL</t>
-  </si>
-  <si>
-    <t>SAP ASE</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>Derby</t>
-  </si>
-  <si>
-    <t>HyperSQL</t>
-  </si>
-  <si>
-    <t>Catalog Term</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>database *2</t>
-  </si>
-  <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>catalog *2</t>
-  </si>
-  <si>
-    <t>CATALOG *2</t>
-  </si>
-  <si>
-    <t>Schema Term</t>
-  </si>
-  <si>
-    <t>schema</t>
-  </si>
-  <si>
-    <t>SCHEMA</t>
-  </si>
-  <si>
-    <t>Identifier default case</t>
-  </si>
-  <si>
-    <t>UPPER</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>Insensitive *3</t>
-  </si>
-  <si>
-    <t>Sensitive *4</t>
-  </si>
-  <si>
-    <t>2. Key Generation</t>
-  </si>
-  <si>
-    <t>Sequences</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Identities generated always</t>
-  </si>
-  <si>
-    <t>Since 12c</t>
-  </si>
-  <si>
-    <t>Identities generated by default</t>
-  </si>
-  <si>
-    <t>Identity columns per table</t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>multiple</t>
-  </si>
-  <si>
-    <t>3. Core Features</t>
-  </si>
-  <si>
-    <t>Top-N rows</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Top-N Rows</t>
-  </si>
-  <si>
-    <t>Query Pagination</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Query Pagination</t>
-  </si>
-  <si>
-    <t>4. Advanced Features</t>
-  </si>
-  <si>
-    <t>With clause supported</t>
-  </si>
-  <si>
-    <t>No?</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Hierarchical Queries</t>
-  </si>
-  <si>
-    <t>Yes *7</t>
-  </si>
-  <si>
-    <t>Since 10.2.2</t>
-  </si>
-  <si>
-    <t>From 8.0</t>
-  </si>
-  <si>
-    <t>Yes *12</t>
-  </si>
-  <si>
-    <t>Constraint Deferrability supported</t>
-  </si>
-  <si>
-    <t>Native ARRAY column type</t>
-  </si>
-  <si>
-    <t>Yes *22</t>
-  </si>
-  <si>
-    <t>Lateral supported</t>
-  </si>
-  <si>
-    <t>Grouping Sets supported</t>
-  </si>
-  <si>
-    <t>Virtual Columns</t>
-  </si>
-  <si>
-    <t>Yes *13</t>
-  </si>
-  <si>
-    <t>No *15</t>
-  </si>
-  <si>
-    <t>Yes *10</t>
-  </si>
-  <si>
-    <t>Since 5.7</t>
-  </si>
-  <si>
-    <t>Yes *18</t>
-  </si>
-  <si>
-    <t>Filter supported</t>
-  </si>
-  <si>
-    <t>Over supported</t>
-  </si>
-  <si>
-    <t>Within supported</t>
-  </si>
-  <si>
-    <t>Temporal Tables</t>
-  </si>
-  <si>
-    <t>Row Pattern Maching supported</t>
-  </si>
-  <si>
-    <t>Full Text Search</t>
-  </si>
-  <si>
-    <t>5. Index Optimization</t>
-  </si>
-  <si>
-    <t>Indexes on Expressions</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Indexes on Expressions</t>
-  </si>
-  <si>
-    <t>Indexes on Expressions with UDF</t>
-  </si>
-  <si>
-    <t>Yes *16</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Indexes on UDF Expressions</t>
-  </si>
-  <si>
-    <t>Descending Indexes</t>
-  </si>
-  <si>
-    <t>No *20</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Descending Indexes</t>
-  </si>
-  <si>
-    <t>Indexes on Virtual Columns</t>
-  </si>
-  <si>
-    <t>Yes *11</t>
-  </si>
-  <si>
-    <t>Yes *19</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Indexes on Virtual Columns</t>
-  </si>
-  <si>
-    <t>Optional indexes on FKs</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - </t>
-  </si>
-  <si>
-    <t>Clustered Index Tables (IOTs, no heap)</t>
-  </si>
-  <si>
-    <t>Yes *9</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Clustered Index Tables</t>
-  </si>
-  <si>
-    <t>Clustering Indexes (separated)</t>
-  </si>
-  <si>
-    <t>Yes *21</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Clustering Index</t>
-  </si>
-  <si>
-    <t>Non-key columns on Indexes</t>
-  </si>
-  <si>
-    <t>Yes *8</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Non-key Columns on Indexes</t>
-  </si>
-  <si>
-    <t>Partial Indexes</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Partial Indexes</t>
-  </si>
-  <si>
-    <t>6. SQL Optimization</t>
-  </si>
-  <si>
-    <t>Explain Plan</t>
-  </si>
-  <si>
-    <t>&lt;database&gt; - Execution Plan</t>
-  </si>
-  <si>
-    <t>Explain Plan without execution</t>
-  </si>
-  <si>
-    <t>Explain Plan with parameters</t>
-  </si>
-  <si>
-    <t>Yes *1</t>
-  </si>
-  <si>
-    <t>Yes *5</t>
-  </si>
-  <si>
-    <t>Yes *6</t>
-  </si>
-  <si>
-    <t>*1 Yes, but requires to specify the type and a value for the parameter, in order to get the explain plan.</t>
-  </si>
-  <si>
-    <t>*2 Informed by the database, but not used internally.</t>
-  </si>
-  <si>
-    <t>*3 The identifier can be typed in any case. It will match other cases.</t>
-  </si>
-  <si>
-    <t>*4 The identifier will be stored in the case it was typed.</t>
-  </si>
-  <si>
-    <t>*5 Yes, but the parameter types must be specified (not the values).</t>
-  </si>
-  <si>
-    <t>*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
-  </si>
-  <si>
-    <t>*7 Recursive CTEs work well. Old fashioned “connect by” queries are not enabled by default (after installation)</t>
-  </si>
-  <si>
-    <t>*8 On unique indexes only.</t>
-  </si>
-  <si>
-    <t>*9 Only on InnoDB tables.</t>
-  </si>
-  <si>
-    <t>*10 Can use user-defined functions since 10.2.1</t>
-  </si>
-  <si>
-    <t>*11 Only persistent virtual columns can be indexed.</t>
-  </si>
-  <si>
-    <t>*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
-  </si>
-  <si>
-    <t>*13 Always persisted.</t>
-  </si>
-  <si>
-    <t>*14 User-defined functions are not allowed.</t>
-  </si>
-  <si>
-    <t>*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
-  </si>
-  <si>
-    <t>*16 Must use deterministic UDFs.</t>
-  </si>
-  <si>
-    <t>*17 (unused)</t>
-  </si>
-  <si>
-    <t>*18 Are always persistent columns.</t>
-  </si>
-  <si>
-    <t>*19 Only on materialized virtual columns.</t>
-  </si>
-  <si>
-    <t>*20 DESC is permitted in the SQL syntax, but ignored.</t>
-  </si>
-  <si>
-    <t>*21 The database does not ensure, but tries to keep the rows in the cluster index order. Periodical maintenance is needed to ensure this ordering.</t>
-  </si>
-  <si>
-    <t>*22 H2 arrays do not have a base type, since they only store Objects.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="126">
+  <si>
+    <t xml:space="preserve">Features \ League</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Tier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subpar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lighweight Tier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MariaDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HyperSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalog Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATALOG *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schema Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier default case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insensitive *3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitive *4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Key Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identities generated always</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 12c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identities generated by default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity columns per table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Core Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top-N rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Top-N Rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Query Pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Query Pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Advanced Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With clause supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hierarchical Queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 10.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 8.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraint Deferrability supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Native ARRAY column type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lateral supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grouping Sets supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No *15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 5.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporal Tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row Pattern Maching supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Text Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Index Optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Indexes on Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Expressions with UDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Indexes on UDF Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descending Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No *20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Descending Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Indexes on Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional indexes on FKs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Index Tables (IOTs, no heap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Clustered Index Tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustering Indexes (separated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Clustering Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-key columns on Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Non-key Columns on Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Partial Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. SQL Optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;database&gt; - Execution Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan without execution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan with parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*1 Yes, but requires to specify the type and a value for the parameter, in order to get the explain plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2 Informed by the database, but not used internally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*3 The identifier can be typed in any case. It will match other cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*4 The identifier will be stored in the case it was typed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*5 Yes, but the parameter types must be specified (not the values).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*8 On unique indexes only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*9 Only on InnoDB tables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*10 Can use user-defined functions since 10.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*13 Always persisted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*14 User-defined functions are not allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*16 Must use deterministic UDFs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*17 (unused)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*18 Are always persistent columns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*19 Only on materialized virtual columns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*20 DESC is permitted in the SQL syntax, but ignored.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*21 The database does not ensure, but tries to keep the rows in the cluster index order. Periodical maintenance is needed to ensure this ordering.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*22 H2 arrays do not have a base type, since they only store Objects.</t>
   </si>
 </sst>
 </file>
@@ -411,7 +405,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -795,22 +789,22 @@
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,25 +1351,25 @@
         <v>33</v>
       </c>
       <c r="C16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="18" t="s">
+      <c r="G16" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="H16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="23" t="s">
         <v>53</v>
-      </c>
-      <c r="H16" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>54</v>
       </c>
       <c r="J16" s="31" t="s">
         <v>34</v>
@@ -1387,7 +1381,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>33</v>
@@ -1423,31 +1417,31 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="33" t="s">
         <v>56</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>57</v>
       </c>
       <c r="J18" s="31" t="s">
         <v>34</v>
@@ -1459,7 +1453,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>33</v>
@@ -1495,7 +1489,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>33</v>
@@ -1531,31 +1525,31 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="D21" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="E21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="18" t="s">
+      <c r="G21" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="H21" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="23" t="s">
         <v>64</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>65</v>
       </c>
       <c r="J21" s="31" t="s">
         <v>34</v>
@@ -1567,7 +1561,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>49</v>
@@ -1603,7 +1597,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>33</v>
@@ -1639,7 +1633,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>33</v>
@@ -1675,7 +1669,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>33</v>
@@ -1711,7 +1705,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>33</v>
@@ -1747,7 +1741,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>49</v>
@@ -1783,7 +1777,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>7</v>
@@ -1819,7 +1813,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>33</v>
@@ -1853,15 +1847,15 @@
       </c>
       <c r="L29" s="0"/>
       <c r="M29" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>34</v>
@@ -1892,30 +1886,30 @@
       </c>
       <c r="L30" s="0"/>
       <c r="M30" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>79</v>
-      </c>
       <c r="G31" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>33</v>
@@ -1927,37 +1921,37 @@
         <v>33</v>
       </c>
       <c r="K31" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L31" s="0"/>
       <c r="M31" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="18" t="s">
+      <c r="G32" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>33</v>
@@ -1970,12 +1964,12 @@
       </c>
       <c r="L32" s="0"/>
       <c r="M32" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>33</v>
@@ -2009,30 +2003,30 @@
       </c>
       <c r="L33" s="0"/>
       <c r="M33" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>88</v>
-      </c>
       <c r="G34" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>33</v>
@@ -2048,21 +2042,21 @@
       </c>
       <c r="L34" s="0"/>
       <c r="M34" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>91</v>
-      </c>
       <c r="D35" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E35" s="30" t="s">
         <v>34</v>
@@ -2087,18 +2081,18 @@
       </c>
       <c r="L35" s="0"/>
       <c r="M35" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="34" t="s">
         <v>93</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>94</v>
       </c>
       <c r="D36" s="28" t="s">
         <v>34</v>
@@ -2126,12 +2120,12 @@
       </c>
       <c r="L36" s="0"/>
       <c r="M36" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>33</v>
@@ -2165,12 +2159,12 @@
       </c>
       <c r="L37" s="0"/>
       <c r="M37" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>7</v>
@@ -2206,7 +2200,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>33</v>
@@ -2240,12 +2234,12 @@
       </c>
       <c r="L39" s="0"/>
       <c r="M39" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>33</v>
@@ -2281,25 +2275,25 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="33" t="s">
+      <c r="E41" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="36" t="s">
+      <c r="F41" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="F41" s="34" t="s">
-        <v>105</v>
-      </c>
       <c r="G41" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H41" s="28" t="s">
         <v>34</v>
@@ -2321,116 +2315,111 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J43" s="0"/>
       <c r="K43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J44" s="37"/>
       <c r="K44" s="37"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2441,7 +2430,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
HOT27 - Reasearch on tuples.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="132">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">multiple</t>
   </si>
   <si>
-    <t xml:space="preserve">3. Core Features</t>
+    <t xml:space="preserve">3a. Core Features</t>
   </si>
   <si>
     <t xml:space="preserve">Top-N rows</t>
@@ -160,10 +160,28 @@
     <t xml:space="preserve">&lt;database&gt; - Query Pagination</t>
   </si>
   <si>
+    <t xml:space="preserve">3b. Tuples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports Tuples Equality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuples [NOT] IN Literal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuples [NOT] IN subqueries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuples in Join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuples inequality</t>
+  </si>
+  <si>
     <t xml:space="preserve">4. Advanced Features</t>
   </si>
   <si>
-    <t xml:space="preserve">With clause supported</t>
+    <t xml:space="preserve">CTEs supported</t>
   </si>
   <si>
     <t xml:space="preserve">No?</t>
@@ -172,7 +190,7 @@
     <t xml:space="preserve">?</t>
   </si>
   <si>
-    <t xml:space="preserve">Hierarchical Queries</t>
+    <t xml:space="preserve">Recursive CTEs supported</t>
   </si>
   <si>
     <t xml:space="preserve">Since 10.2.2</t>
@@ -787,24 +805,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="8.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="1" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,8 +1328,8 @@
       <c r="A15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>33</v>
+      <c r="B15" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>33</v>
@@ -1320,56 +1337,56 @@
       <c r="D15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>49</v>
+      <c r="E15" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="L15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>33</v>
+      <c r="C16" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>33</v>
+      <c r="E16" s="30" t="s">
+        <v>34</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>34</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="J16" s="31" t="s">
         <v>34</v>
@@ -1381,13 +1398,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>34</v>
+      <c r="C17" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>33</v>
@@ -1395,11 +1412,11 @@
       <c r="E17" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>34</v>
+      <c r="F17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>34</v>
@@ -1410,20 +1427,20 @@
       <c r="J17" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="K17" s="32" t="s">
-        <v>34</v>
+      <c r="K17" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="L17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>33</v>
@@ -1431,17 +1448,17 @@
       <c r="E18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>34</v>
+      <c r="F18" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="H18" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="33" t="s">
-        <v>56</v>
+      <c r="I18" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="J18" s="31" t="s">
         <v>34</v>
@@ -1453,10 +1470,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>33</v>
@@ -1464,212 +1481,212 @@
       <c r="D19" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>49</v>
+      <c r="E19" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="L19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>49</v>
+      <c r="A20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="L20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>61</v>
+        <v>33</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="32" t="s">
-        <v>34</v>
+      <c r="F21" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="L21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>49</v>
+      <c r="E22" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>33</v>
+      <c r="C23" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>49</v>
+      <c r="E23" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>49</v>
+      <c r="C24" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>49</v>
+      <c r="E24" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="L24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>33</v>
@@ -1677,137 +1694,137 @@
       <c r="C25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>49</v>
+      <c r="D25" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="J25" s="21" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="26" t="s">
-        <v>49</v>
+      <c r="C26" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="J26" s="21" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J27" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K27" s="22" t="s">
-        <v>49</v>
+      <c r="J27" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="L27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>16</v>
+      <c r="B28" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="L28" s="0"/>
     </row>
@@ -1824,74 +1841,68 @@
       <c r="D29" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J29" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>34</v>
+      <c r="E29" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="L29" s="0"/>
-      <c r="M29" s="0" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" s="32" t="s">
-        <v>34</v>
+      <c r="E30" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K30" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="L30" s="0"/>
-      <c r="M30" s="0" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>33</v>
@@ -1899,164 +1910,152 @@
       <c r="C31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K31" s="27" t="s">
-        <v>78</v>
+      <c r="D31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K31" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="L31" s="0"/>
-      <c r="M31" s="0" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="I32" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" s="32" t="s">
-        <v>34</v>
+      <c r="C32" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K32" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="L32" s="0"/>
-      <c r="M32" s="0" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" s="32" t="s">
-        <v>34</v>
+        <v>76</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K33" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="L33" s="0"/>
-      <c r="M33" s="0" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I34" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J34" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" s="32" t="s">
-        <v>34</v>
+      <c r="A34" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="L34" s="0"/>
-      <c r="M34" s="0" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>90</v>
+        <v>78</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="E35" s="30" t="s">
         <v>34</v>
@@ -2067,8 +2066,8 @@
       <c r="G35" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="28" t="s">
-        <v>34</v>
+      <c r="H35" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="I35" s="29" t="s">
         <v>34</v>
@@ -2081,24 +2080,24 @@
       </c>
       <c r="L35" s="0"/>
       <c r="M35" s="0" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>33</v>
+        <v>80</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>34</v>
       </c>
       <c r="F36" s="27" t="s">
         <v>34</v>
@@ -2106,8 +2105,8 @@
       <c r="G36" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H36" s="28" t="s">
-        <v>34</v>
+      <c r="H36" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="I36" s="29" t="s">
         <v>34</v>
@@ -2120,12 +2119,12 @@
       </c>
       <c r="L36" s="0"/>
       <c r="M36" s="0" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>33</v>
@@ -2140,67 +2139,70 @@
         <v>33</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J37" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K37" s="32" t="s">
-        <v>34</v>
+        <v>84</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>84</v>
       </c>
       <c r="L37" s="0"/>
       <c r="M37" s="0" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>16</v>
+      <c r="A38" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K38" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="L38" s="0"/>
+      <c r="M38" s="0" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>33</v>
@@ -2214,166 +2216,367 @@
       <c r="E39" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>33</v>
+      <c r="F39" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="H39" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="I39" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J39" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K39" s="25" t="s">
-        <v>33</v>
+      <c r="I39" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="L39" s="0"/>
       <c r="M39" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>33</v>
+      <c r="C40" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="E40" s="17" t="s">
         <v>33</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="H40" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="23" t="s">
-        <v>33</v>
+      <c r="I40" s="29" t="s">
+        <v>34</v>
       </c>
       <c r="J40" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="K40" s="25" t="s">
-        <v>33</v>
+      <c r="K40" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="L40" s="0"/>
+      <c r="M40" s="0" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="L41" s="0"/>
+      <c r="M41" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="L42" s="0"/>
+      <c r="M42" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="33" t="s">
+      <c r="B43" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K43" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="L43" s="0"/>
+      <c r="M43" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="E41" s="36" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="B44" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G41" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="H41" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I41" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J41" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K41" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="L41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J42" s="0"/>
-      <c r="K42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="B45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="J43" s="0"/>
-      <c r="K43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="B46" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I46" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J46" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K46" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="B47" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="33" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="E47" s="36" t="s">
         <v>109</v>
       </c>
+      <c r="F47" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G47" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J47" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K47" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>110</v>
-      </c>
+      <c r="J48" s="0"/>
+      <c r="K48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="J49" s="0"/>
+      <c r="K49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>111</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2420,6 +2623,36 @@
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2430,7 +2663,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
HOT-38 - Mixed-case identifiers complete.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">High End</t>
   </si>
   <si>
-    <t xml:space="preserve">Superior</t>
+    <t xml:space="preserve">Outstanding</t>
   </si>
   <si>
     <t xml:space="preserve">Middle Tier</t>
@@ -803,22 +803,22 @@
   </sheetPr>
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="1" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,7 +2696,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Adding virtual columns summary.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="126">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -253,6 +253,9 @@
     <t xml:space="preserve">Indexes on Expressions</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes *7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indexes on Expressions with UDF</t>
   </si>
   <si>
@@ -349,6 +352,9 @@
     <t xml:space="preserve">*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
   </si>
   <si>
+    <t xml:space="preserve">*7 Expressions must be enclosed in parenthesis</t>
+  </si>
+  <si>
     <t xml:space="preserve">*8 On unique indexes only.</t>
   </si>
   <si>
@@ -358,7 +364,7 @@
     <t xml:space="preserve">*10 Can use user-defined functions since 10.2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
+    <t xml:space="preserve">*11 Only persistent virtual columns can be indexed. But... I could index virtual columns too (?).</t>
   </si>
   <si>
     <t xml:space="preserve">*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
@@ -767,22 +773,22 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="1" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2010,7 +2016,7 @@
         <v>33</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>34</v>
@@ -2037,10 +2043,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>34</v>
@@ -2073,7 +2079,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>33</v>
@@ -2088,10 +2094,10 @@
         <v>33</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H37" s="16" t="s">
         <v>33</v>
@@ -2103,13 +2109,13 @@
         <v>33</v>
       </c>
       <c r="K37" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>33</v>
@@ -2124,13 +2130,13 @@
         <v>33</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>33</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I38" s="21" t="s">
         <v>33</v>
@@ -2145,7 +2151,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>33</v>
@@ -2181,7 +2187,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>33</v>
@@ -2196,10 +2202,10 @@
         <v>33</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H40" s="16" t="s">
         <v>33</v>
@@ -2217,16 +2223,16 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E41" s="25" t="s">
         <v>34</v>
@@ -2253,13 +2259,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>34</v>
@@ -2289,7 +2295,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>33</v>
@@ -2325,7 +2331,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>7</v>
@@ -2361,7 +2367,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>33</v>
@@ -2397,7 +2403,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>33</v>
@@ -2433,7 +2439,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>33</v>
@@ -2442,16 +2448,16 @@
         <v>33</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F47" s="31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G47" s="31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H47" s="25" t="s">
         <v>34</v>
@@ -2469,37 +2475,37 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C48" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="E48" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H48" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I48" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="J48" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="I48" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="J48" s="22" t="s">
+      <c r="K48" s="23" t="s">
         <v>101</v>
-      </c>
-      <c r="K48" s="23" t="s">
-        <v>100</v>
       </c>
       <c r="L48" s="0"/>
     </row>
@@ -2509,111 +2515,116 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J50" s="0"/>
       <c r="K50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J51" s="33"/>
       <c r="K51" s="33"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2624,7 +2635,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Cursor tests on Oracle, DB2, PostgreSQL, SQL Server, MariabDB, MySQL.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="134">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -124,6 +124,9 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
+    <t xml:space="preserve">Since 10.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
     <t xml:space="preserve">Since 12c</t>
   </si>
   <si>
+    <t xml:space="preserve">Since 10.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identities generated by default</t>
   </si>
   <si>
@@ -172,6 +178,27 @@
     <t xml:space="preserve">Tuples inequality</t>
   </si>
   <si>
+    <t xml:space="preserve">3c. Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window Functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 10.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 8.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grouping Sets supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within supported</t>
+  </si>
+  <si>
     <t xml:space="preserve">4. Advanced Features</t>
   </si>
   <si>
@@ -181,21 +208,12 @@
     <t xml:space="preserve">Since 10.2.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Since 8.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recursive CTEs supported</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *12</t>
   </si>
   <si>
-    <t xml:space="preserve">Over supported (windowing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since 10.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Virtual Columns</t>
   </si>
   <si>
@@ -217,6 +235,15 @@
     <t xml:space="preserve">Constraint Deferrability supported</t>
   </si>
   <si>
+    <t xml:space="preserve">Select fetch size supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes*23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes*24</t>
+  </si>
+  <si>
     <t xml:space="preserve">Native ARRAY column type</t>
   </si>
   <si>
@@ -229,22 +256,10 @@
     <t xml:space="preserve">Lateral outer join</t>
   </si>
   <si>
-    <t xml:space="preserve">Grouping Sets supported</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter supported</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within supported</t>
-  </si>
-  <si>
     <t xml:space="preserve">Temporal Tables</t>
   </si>
   <si>
-    <t xml:space="preserve">Row Pattern Maching supported</t>
+    <t xml:space="preserve">Row Pattern Matching supported</t>
   </si>
   <si>
     <t xml:space="preserve">Full Text Search</t>
@@ -289,7 +304,7 @@
     <t xml:space="preserve">Yes *9</t>
   </si>
   <si>
-    <t xml:space="preserve">Clustering Indexes (separated)</t>
+    <t xml:space="preserve">Clustering Indexes</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *21</t>
@@ -400,7 +415,13 @@
     <t xml:space="preserve">*21 The database does not ensure, but tries to keep the rows in the cluster index order. Periodical maintenance is needed to ensure this ordering.</t>
   </si>
   <si>
-    <t xml:space="preserve">*22 H2 arrays do not have a base type, since they only store Objects.</t>
+    <t xml:space="preserve">*22 H2 arrays do not have a base type. They only store Java Objects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*23 Yes, but not efficient. If the fetch size is &gt; 0, then it first materializes the entire query on the server side, then streams it. Otherwise the fetch size is ignored.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*24 Yes, but not efficient. If the fetch size is &gt; 0, then it first materializes the entire query on the server side, then streams it. Otherwise the fetch size is ignored.</t>
   </si>
 </sst>
 </file>
@@ -410,7 +431,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -435,13 +456,6 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCE181E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -560,7 +574,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -677,15 +691,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -710,7 +720,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFE6E6FF"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -774,23 +784,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,14 +1027,14 @@
       <c r="E7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="17" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I7" s="21" t="s">
         <v>33</v>
@@ -1037,31 +1049,31 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>34</v>
+      <c r="D8" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>33</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J8" s="22" t="s">
         <v>33</v>
@@ -1073,11 +1085,11 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>36</v>
-      </c>
       <c r="C9" s="17" t="s">
         <v>33</v>
       </c>
@@ -1085,7 +1097,7 @@
         <v>33</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>33</v>
@@ -1094,7 +1106,7 @@
         <v>33</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I9" s="21" t="s">
         <v>33</v>
@@ -1109,43 +1121,43 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -1181,7 +1193,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>33</v>
@@ -1217,7 +1229,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>33</v>
@@ -1238,7 +1250,7 @@
         <v>33</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I13" s="21" t="s">
         <v>33</v>
@@ -1253,7 +1265,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>7</v>
@@ -1289,10 +1301,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>33</v>
@@ -1301,7 +1313,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>33</v>
@@ -1310,13 +1322,13 @@
         <v>33</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I15" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K15" s="23" t="s">
         <v>33</v>
@@ -1325,19 +1337,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" s="17" t="s">
         <v>33</v>
@@ -1346,13 +1358,13 @@
         <v>33</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I16" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K16" s="23" t="s">
         <v>33</v>
@@ -1361,7 +1373,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>33</v>
@@ -1373,7 +1385,7 @@
         <v>33</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>33</v>
@@ -1382,13 +1394,13 @@
         <v>33</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K17" s="23" t="s">
         <v>33</v>
@@ -1397,10 +1409,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>33</v>
@@ -1409,7 +1421,7 @@
         <v>33</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>33</v>
@@ -1418,13 +1430,13 @@
         <v>33</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K18" s="23" t="s">
         <v>33</v>
@@ -1433,10 +1445,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>33</v>
@@ -1445,7 +1457,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>33</v>
@@ -1454,13 +1466,13 @@
         <v>33</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I19" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K19" s="23" t="s">
         <v>33</v>
@@ -1469,7 +1481,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>7</v>
@@ -1505,7 +1517,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>33</v>
@@ -1520,28 +1532,28 @@
         <v>33</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="L21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>33</v>
@@ -1555,60 +1567,30 @@
       <c r="E22" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="23" t="s">
-        <v>33</v>
-      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>33</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" s="28" t="s">
-        <v>34</v>
-      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,101 +1600,85 @@
       <c r="B24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K24" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="L24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K25" s="28" t="s">
-        <v>34</v>
+      <c r="B25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="L25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>34</v>
+      <c r="C26" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>34</v>
+      <c r="E26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>66</v>
+        <v>35</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K26" s="23" t="s">
         <v>33</v>
@@ -1721,7 +1687,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>33</v>
@@ -1735,95 +1701,95 @@
       <c r="E27" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>34</v>
+      <c r="F27" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K27" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="L27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="26" t="s">
-        <v>34</v>
+      <c r="H28" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K28" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30" t="s">
-        <v>69</v>
+      <c r="A29" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>33</v>
+      <c r="C29" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J29" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="K29" s="20" t="s">
-        <v>70</v>
+      <c r="E29" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="L29" s="0"/>
     </row>
@@ -1831,77 +1797,69 @@
       <c r="A30" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>70</v>
+      <c r="B30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J30" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="K30" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="E30" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="15"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="20"/>
       <c r="L30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>70</v>
+      <c r="C31" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J31" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="K31" s="20" t="s">
-        <v>70</v>
+      <c r="E31" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="L31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>33</v>
@@ -1909,215 +1867,161 @@
       <c r="C32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J32" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="K32" s="20" t="s">
-        <v>70</v>
+      <c r="D32" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="L32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J33" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="K33" s="20" t="s">
-        <v>70</v>
+      <c r="C33" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="L33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J34" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="K34" s="20" t="s">
-        <v>70</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="A35" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="20"/>
       <c r="L35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I36" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K36" s="28" t="s">
-        <v>34</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="20"/>
       <c r="L36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="J37" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K37" s="28" t="s">
-        <v>34</v>
+      <c r="A37" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="L37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>33</v>
@@ -2126,64 +2030,64 @@
         <v>33</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>33</v>
+        <v>83</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="H38" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I38" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J38" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="K38" s="24" t="s">
-        <v>82</v>
+      <c r="I38" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="L38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>33</v>
+        <v>85</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>33</v>
+        <v>33</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="J39" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K39" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L39" s="0"/>
     </row>
@@ -2204,208 +2108,208 @@
         <v>33</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="H40" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="J40" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K40" s="28" t="s">
-        <v>34</v>
+      <c r="I40" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="L40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="24" t="s">
-        <v>34</v>
+      <c r="C41" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I41" s="26" t="s">
-        <v>34</v>
+        <v>90</v>
+      </c>
+      <c r="I41" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K41" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>34</v>
+        <v>91</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="I42" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J42" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K42" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="31" t="s">
         <v>92</v>
       </c>
+      <c r="B43" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="D43" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H43" s="25" t="s">
-        <v>34</v>
+      <c r="F43" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="I43" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K43" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>33</v>
+        <v>94</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H44" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I44" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K44" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>16</v>
+      <c r="A45" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J45" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K45" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="L45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>33</v>
@@ -2419,65 +2323,65 @@
       <c r="E46" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I46" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J46" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="K46" s="23" t="s">
-        <v>33</v>
+      <c r="F46" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J46" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K46" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="L46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J47" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K47" s="23" t="s">
-        <v>33</v>
+      <c r="A47" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="L47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>33</v>
@@ -2485,26 +2389,26 @@
       <c r="C48" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="F48" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="G48" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="H48" s="25" t="s">
-        <v>34</v>
+      <c r="D48" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="I48" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="J48" s="27" t="s">
-        <v>34</v>
+      <c r="J48" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="K48" s="23" t="s">
         <v>33</v>
@@ -2516,153 +2420,235 @@
         <v>101</v>
       </c>
       <c r="B49" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I49" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K49" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="L49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="B50" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="H49" s="16" t="s">
+      <c r="E50" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="I49" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="J49" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="L49" s="0"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J50" s="0"/>
-      <c r="K50" s="0"/>
+      <c r="F50" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G50" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I50" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J50" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K50" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="L50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="J51" s="0"/>
-      <c r="K51" s="0"/>
+      <c r="A51" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I51" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="J51" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="K51" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="L51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="J52" s="33"/>
-      <c r="K52" s="33"/>
+      <c r="J52" s="0"/>
+      <c r="K52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>107</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="J53" s="0"/>
+      <c r="K53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>108</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Execution Plan Renderer Engine started.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="161">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes *8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 11.0</t>
   </si>
   <si>
     <t xml:space="preserve">Partial Indexes</t>
@@ -652,7 +655,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -773,14 +776,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -876,22 +871,23 @@
   </sheetPr>
   <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D66" activeCellId="0" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,10 +2026,10 @@
       <c r="A34" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
@@ -2082,10 +2078,10 @@
       <c r="A36" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
@@ -2132,7 +2128,7 @@
       <c r="C38" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="31"/>
+      <c r="D38" s="15"/>
       <c r="E38" s="29" t="s">
         <v>63</v>
       </c>
@@ -2189,9 +2185,9 @@
       <c r="B40" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
@@ -2236,10 +2232,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
@@ -2250,10 +2246,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
@@ -2264,10 +2260,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
       <c r="H44" s="15"/>
@@ -2426,10 +2422,10 @@
       <c r="E50" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="32" t="s">
+      <c r="F50" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="G50" s="32" t="s">
+      <c r="G50" s="30" t="s">
         <v>91</v>
       </c>
       <c r="H50" s="15"/>
@@ -2463,7 +2459,7 @@
       <c r="H51" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I51" s="33" t="s">
+      <c r="I51" s="31" t="s">
         <v>93</v>
       </c>
       <c r="J51" s="27" t="s">
@@ -2859,10 +2855,10 @@
       <c r="B64" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="D64" s="34" t="s">
+      <c r="D64" s="32" t="s">
         <v>113</v>
       </c>
       <c r="E64" s="25" t="s">
@@ -2895,11 +2891,11 @@
       <c r="B65" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="D65" s="25" t="s">
-        <v>35</v>
+      <c r="D65" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="E65" s="16" t="s">
         <v>33</v>
@@ -2926,7 +2922,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B66" s="17" t="s">
         <v>33</v>
@@ -2962,7 +2958,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>7</v>
@@ -2998,7 +2994,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B68" s="17" t="s">
         <v>33</v>
@@ -3034,7 +3030,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>33</v>
@@ -3070,7 +3066,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B70" s="17" t="s">
         <v>33</v>
@@ -3078,17 +3074,17 @@
       <c r="C70" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="E70" s="33" t="s">
+      <c r="D70" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="F70" s="32" t="s">
+      <c r="E70" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="G70" s="32" t="s">
-        <v>123</v>
+      <c r="F70" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="G70" s="30" t="s">
+        <v>124</v>
       </c>
       <c r="H70" s="25" t="s">
         <v>35</v>
@@ -3106,37 +3102,37 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C71" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D71" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D71" s="16" t="s">
-        <v>125</v>
-      </c>
       <c r="E71" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H71" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="I71" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="J71" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="I71" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="J71" s="22" t="s">
+      <c r="K71" s="23" t="s">
         <v>126</v>
-      </c>
-      <c r="K71" s="23" t="s">
-        <v>125</v>
       </c>
       <c r="L71" s="0"/>
     </row>
@@ -3154,7 +3150,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B73" s="0"/>
       <c r="C73" s="0"/>
@@ -3169,7 +3165,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B74" s="0"/>
       <c r="C74" s="0"/>
@@ -3179,12 +3175,12 @@
       <c r="G74" s="0"/>
       <c r="H74" s="0"/>
       <c r="I74" s="0"/>
-      <c r="J74" s="35"/>
-      <c r="K74" s="35"/>
+      <c r="J74" s="33"/>
+      <c r="K74" s="33"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B75" s="0"/>
       <c r="C75" s="0"/>
@@ -3199,7 +3195,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B76" s="0"/>
       <c r="C76" s="0"/>
@@ -3214,7 +3210,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B77" s="0"/>
       <c r="C77" s="0"/>
@@ -3229,7 +3225,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
@@ -3244,7 +3240,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B79" s="0"/>
       <c r="C79" s="0"/>
@@ -3259,7 +3255,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B80" s="0"/>
       <c r="C80" s="0"/>
@@ -3274,7 +3270,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
@@ -3289,7 +3285,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B82" s="0"/>
       <c r="C82" s="0"/>
@@ -3304,7 +3300,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B83" s="0"/>
       <c r="C83" s="0"/>
@@ -3319,7 +3315,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B84" s="0"/>
       <c r="C84" s="0"/>
@@ -3334,7 +3330,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B85" s="0"/>
       <c r="C85" s="0"/>
@@ -3349,7 +3345,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B86" s="0"/>
       <c r="C86" s="0"/>
@@ -3364,7 +3360,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B87" s="0"/>
       <c r="C87" s="0"/>
@@ -3379,7 +3375,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B88" s="0"/>
       <c r="C88" s="0"/>
@@ -3394,7 +3390,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B89" s="0"/>
       <c r="C89" s="0"/>
@@ -3409,7 +3405,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B90" s="0"/>
       <c r="C90" s="0"/>
@@ -3424,7 +3420,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B91" s="0"/>
       <c r="C91" s="0"/>
@@ -3439,7 +3435,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B92" s="0"/>
       <c r="C92" s="0"/>
@@ -3454,7 +3450,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B93" s="0"/>
       <c r="C93" s="0"/>
@@ -3469,7 +3465,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B94" s="0"/>
       <c r="C94" s="0"/>
@@ -3484,7 +3480,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
@@ -3499,7 +3495,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B96" s="0"/>
       <c r="C96" s="0"/>
@@ -3586,7 +3582,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>7</v>
@@ -3621,42 +3617,42 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K104" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B105" s="24" t="s">
         <v>35</v>
@@ -3671,10 +3667,10 @@
         <v>35</v>
       </c>
       <c r="F105" s="24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G105" s="24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H105" s="24" t="s">
         <v>35</v>
@@ -3691,25 +3687,25 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B106" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C106" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D106" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F106" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="B106" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C106" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D106" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E106" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F106" s="24" t="s">
-        <v>156</v>
-      </c>
       <c r="G106" s="24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H106" s="17" t="s">
         <v>33</v>
@@ -3726,12 +3722,12 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented natural and union joins.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database-comparison.xlsx
+++ b/hotrod/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="172">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t xml:space="preserve">Tuples inequality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL:1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNION Join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
   </si>
   <si>
     <t xml:space="preserve">SQL:1999</t>
@@ -679,7 +688,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -788,6 +797,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -889,10 +902,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J71" activeCellId="0" sqref="J71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1665,142 +1678,157 @@
       <c r="A21" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="16" t="s">
+      <c r="B21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="I21" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K21" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L21" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" s="22" t="s">
-        <v>35</v>
+      <c r="B22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="H23" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="22" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>18</v>
+      <c r="B24" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>35</v>
@@ -1814,245 +1842,233 @@
       <c r="E25" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L25" s="22" t="s">
-        <v>35</v>
-      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="28" t="s">
+      <c r="B27" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J26" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="K26" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="I27" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J27" s="28" t="s">
-        <v>67</v>
+      <c r="G27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="26" t="s">
+        <v>37</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>67</v>
+        <v>37</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="28" t="s">
+      <c r="C28" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" s="28" t="s">
-        <v>67</v>
+      <c r="G28" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="19"/>
+      <c r="B29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
+      <c r="B30" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L31" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="I32" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J32" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="K32" s="28" t="s">
-        <v>67</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>8</v>
@@ -2090,22 +2106,42 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="K34" s="29" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>8</v>
@@ -2143,7 +2179,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2157,49 +2193,52 @@
       <c r="K36" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="19"/>
+      <c r="A37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>66</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="14"/>
-      <c r="E38" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>66</v>
-      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="14"/>
       <c r="I38" s="17"/>
@@ -2207,54 +2246,49 @@
       <c r="K38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A39" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H39" s="14"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="19"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="B40" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>69</v>
+      </c>
       <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="13"/>
+      <c r="E40" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>69</v>
+      </c>
       <c r="G40" s="13"/>
       <c r="H40" s="14"/>
       <c r="I40" s="17"/>
@@ -2262,162 +2296,152 @@
       <c r="K40" s="19"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="19"/>
+      <c r="A41" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="7" t="s">
+      <c r="A42" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="19"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="19"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G44" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H44" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="9" t="s">
+      <c r="I44" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="J44" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K42" s="11" t="s">
+      <c r="K44" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L42" s="9" t="s">
+      <c r="L44" s="9" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I43" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J43" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K43" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L43" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F44" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I44" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J44" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K44" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L44" s="23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G45" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="29" t="s">
+      <c r="H45" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="G45" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="H45" s="14"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="19"/>
+      <c r="J45" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" s="23" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>35</v>
@@ -2440,50 +2464,45 @@
       <c r="H46" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I46" s="30" t="s">
-        <v>96</v>
+      <c r="I46" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="J46" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K46" s="22" t="s">
-        <v>35</v>
+      <c r="K46" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F47" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H47" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I47" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J47" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K47" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="H47" s="14"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="19"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
@@ -2498,8 +2517,8 @@
       <c r="D48" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>35</v>
+      <c r="E48" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="F48" s="23" t="s">
         <v>37</v>
@@ -2510,19 +2529,19 @@
       <c r="H48" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I48" s="25" t="s">
-        <v>37</v>
+      <c r="I48" s="31" t="s">
+        <v>99</v>
       </c>
       <c r="J48" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K48" s="27" t="s">
-        <v>37</v>
+      <c r="K48" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>35</v>
@@ -2530,38 +2549,76 @@
       <c r="C49" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="19"/>
+      <c r="D49" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I49" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J49" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K49" s="28" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="19"/>
+      <c r="C50" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G50" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I50" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J50" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K50" s="28" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
+        <v>102</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="13"/>
@@ -2572,198 +2629,154 @@
       <c r="K51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I52" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L52" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A52" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D53" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F53" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I53" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J53" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K53" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L53" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F54" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G54" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I54" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J54" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K54" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L54" s="27" t="s">
-        <v>37</v>
+      <c r="B54" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L54" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>35</v>
+      <c r="E55" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="H55" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I55" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J55" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K55" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="L55" s="27" t="s">
+      <c r="I55" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J55" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K55" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L55" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D56" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G56" s="16" t="s">
-        <v>35</v>
+      <c r="C56" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="I56" s="20" t="s">
-        <v>35</v>
+        <v>35</v>
+      </c>
+      <c r="I56" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="J56" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K56" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L56" s="27" t="s">
+      <c r="K56" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L56" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>35</v>
@@ -2778,59 +2791,62 @@
         <v>35</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="H57" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I57" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J57" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K57" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L57" s="15" t="s">
-        <v>35</v>
+      <c r="I57" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="L57" s="28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F58" s="16" t="s">
+      <c r="G58" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H58" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G58" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I58" s="25" t="s">
-        <v>37</v>
+      <c r="I58" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="J58" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K58" s="27" t="s">
+      <c r="K58" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L58" s="28" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2838,17 +2854,17 @@
       <c r="A59" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>37</v>
+      <c r="B59" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="F59" s="23" t="s">
         <v>37</v>
@@ -2856,8 +2872,8 @@
       <c r="G59" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H59" s="24" t="s">
-        <v>37</v>
+      <c r="H59" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="I59" s="25" t="s">
         <v>37</v>
@@ -2865,34 +2881,37 @@
       <c r="J59" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K59" s="27" t="s">
-        <v>37</v>
+      <c r="K59" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L59" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F60" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G60" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H60" s="24" t="s">
-        <v>37</v>
+      <c r="G60" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="I60" s="25" t="s">
         <v>37</v>
@@ -2900,89 +2919,83 @@
       <c r="J60" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K60" s="27" t="s">
+      <c r="K60" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H61" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I61" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J61" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K61" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F61" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G61" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H61" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I61" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J61" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K61" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L61" s="27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="6" t="s">
+      <c r="B62" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I62" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J62" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K62" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L62" s="9" t="s">
-        <v>18</v>
+      <c r="D62" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H62" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I62" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J62" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K62" s="28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>35</v>
@@ -2996,67 +3009,69 @@
       <c r="E63" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H63" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I63" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J63" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K63" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L63" s="22" t="s">
-        <v>35</v>
+      <c r="F63" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H63" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I63" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J63" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K63" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L63" s="28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G64" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H64" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I64" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J64" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K64" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L64" s="19"/>
+      <c r="A64" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K64" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L64" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B65" s="16" t="s">
         <v>35</v>
@@ -3064,180 +3079,230 @@
       <c r="C65" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="E65" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="F65" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G65" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="H65" s="24" t="s">
-        <v>37</v>
+      <c r="D65" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="I65" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J65" s="26" t="s">
-        <v>37</v>
+      <c r="J65" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="K65" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L65" s="26" t="s">
-        <v>37</v>
+      <c r="L65" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I66" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K66" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L66" s="19"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="E67" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="F67" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="D66" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F66" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="H66" s="15" t="s">
+      <c r="G67" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="H67" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I67" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K67" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L67" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="I66" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="J66" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="K66" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="L66" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0"/>
-      <c r="C67" s="0"/>
-      <c r="D67" s="0"/>
-      <c r="E67" s="0"/>
-      <c r="F67" s="0"/>
-      <c r="G67" s="0"/>
-      <c r="H67" s="0"/>
-      <c r="I67" s="0"/>
-      <c r="J67" s="0"/>
-      <c r="K67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="s">
+      <c r="B68" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="C68" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G68" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I68" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="J68" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K68" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="L68" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0"/>
+      <c r="C69" s="0"/>
+      <c r="D69" s="0"/>
+      <c r="E69" s="0"/>
+      <c r="F69" s="0"/>
+      <c r="G69" s="0"/>
+      <c r="H69" s="0"/>
+      <c r="I69" s="0"/>
+      <c r="J69" s="0"/>
+      <c r="K69" s="0"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="D70" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F70" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H68" s="8" t="s">
+      <c r="H70" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I68" s="9" t="s">
+      <c r="I70" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J68" s="10" t="s">
+      <c r="J70" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K68" s="11" t="s">
+      <c r="K70" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L68" s="9" t="s">
+      <c r="L70" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C69" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E69" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F69" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="G69" s="23" t="s">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="F71" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="G71" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H69" s="23" t="s">
+      <c r="H71" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I69" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="J69" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="K69" s="29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0"/>
-      <c r="C70" s="0"/>
-      <c r="D70" s="0"/>
-      <c r="E70" s="0"/>
-      <c r="F70" s="0"/>
-      <c r="G70" s="0"/>
-      <c r="H70" s="0"/>
-      <c r="I70" s="0"/>
-      <c r="J70" s="0"/>
-      <c r="K70" s="0"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0"/>
-      <c r="C71" s="0"/>
-      <c r="D71" s="0"/>
-      <c r="E71" s="0"/>
-      <c r="F71" s="0"/>
-      <c r="G71" s="0"/>
-      <c r="H71" s="0"/>
-      <c r="I71" s="0"/>
-      <c r="J71" s="0"/>
-      <c r="K71" s="0"/>
+      <c r="I71" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="J71" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="K71" s="30" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0"/>
@@ -3252,9 +3317,6 @@
       <c r="K72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>136</v>
-      </c>
       <c r="B73" s="0"/>
       <c r="C73" s="0"/>
       <c r="D73" s="0"/>
@@ -3267,9 +3329,6 @@
       <c r="K73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>137</v>
-      </c>
       <c r="B74" s="0"/>
       <c r="C74" s="0"/>
       <c r="D74" s="0"/>
@@ -3278,12 +3337,12 @@
       <c r="G74" s="0"/>
       <c r="H74" s="0"/>
       <c r="I74" s="0"/>
-      <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
+      <c r="J74" s="0"/>
+      <c r="K74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B75" s="0"/>
       <c r="C75" s="0"/>
@@ -3298,7 +3357,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B76" s="0"/>
       <c r="C76" s="0"/>
@@ -3308,12 +3367,12 @@
       <c r="G76" s="0"/>
       <c r="H76" s="0"/>
       <c r="I76" s="0"/>
-      <c r="J76" s="0"/>
-      <c r="K76" s="0"/>
+      <c r="J76" s="33"/>
+      <c r="K76" s="33"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B77" s="0"/>
       <c r="C77" s="0"/>
@@ -3328,7 +3387,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
@@ -3343,7 +3402,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B79" s="0"/>
       <c r="C79" s="0"/>
@@ -3358,7 +3417,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B80" s="0"/>
       <c r="C80" s="0"/>
@@ -3373,7 +3432,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
@@ -3388,7 +3447,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B82" s="0"/>
       <c r="C82" s="0"/>
@@ -3403,7 +3462,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B83" s="0"/>
       <c r="C83" s="0"/>
@@ -3418,7 +3477,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B84" s="0"/>
       <c r="C84" s="0"/>
@@ -3433,7 +3492,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B85" s="0"/>
       <c r="C85" s="0"/>
@@ -3448,7 +3507,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B86" s="0"/>
       <c r="C86" s="0"/>
@@ -3463,7 +3522,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B87" s="0"/>
       <c r="C87" s="0"/>
@@ -3478,7 +3537,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B88" s="0"/>
       <c r="C88" s="0"/>
@@ -3493,7 +3552,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B89" s="0"/>
       <c r="C89" s="0"/>
@@ -3508,7 +3567,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B90" s="0"/>
       <c r="C90" s="0"/>
@@ -3523,7 +3582,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B91" s="0"/>
       <c r="C91" s="0"/>
@@ -3538,7 +3597,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B92" s="0"/>
       <c r="C92" s="0"/>
@@ -3553,7 +3612,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B93" s="0"/>
       <c r="C93" s="0"/>
@@ -3568,7 +3627,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B94" s="0"/>
       <c r="C94" s="0"/>
@@ -3583,7 +3642,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
@@ -3598,7 +3657,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B96" s="0"/>
       <c r="C96" s="0"/>
@@ -3613,7 +3672,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B97" s="0"/>
       <c r="C97" s="0"/>
@@ -3627,6 +3686,9 @@
       <c r="K97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>162</v>
+      </c>
       <c r="B98" s="0"/>
       <c r="C98" s="0"/>
       <c r="D98" s="0"/>
@@ -3639,6 +3701,9 @@
       <c r="K98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>163</v>
+      </c>
       <c r="B99" s="0"/>
       <c r="C99" s="0"/>
       <c r="D99" s="0"/>
@@ -3687,153 +3752,177 @@
       <c r="K102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="0"/>
+      <c r="C103" s="0"/>
+      <c r="D103" s="0"/>
+      <c r="E103" s="0"/>
+      <c r="F103" s="0"/>
+      <c r="G103" s="0"/>
+      <c r="H103" s="0"/>
+      <c r="I103" s="0"/>
+      <c r="J103" s="0"/>
+      <c r="K103" s="0"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="0"/>
+      <c r="C104" s="0"/>
+      <c r="D104" s="0"/>
+      <c r="E104" s="0"/>
+      <c r="F104" s="0"/>
+      <c r="G104" s="0"/>
+      <c r="H104" s="0"/>
+      <c r="I104" s="0"/>
+      <c r="J104" s="0"/>
+      <c r="K104" s="0"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B105" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C105" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D103" s="8" t="s">
+      <c r="D105" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E103" s="8" t="s">
+      <c r="E105" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F103" s="7" t="s">
+      <c r="F105" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G103" s="7" t="s">
+      <c r="G105" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H103" s="8" t="s">
+      <c r="H105" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I103" s="9" t="s">
+      <c r="I105" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J103" s="10" t="s">
+      <c r="J105" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K103" s="11" t="s">
+      <c r="K105" s="11" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="F104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="G104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="H104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="I104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="J104" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="K104" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B105" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C105" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D105" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E105" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F105" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="G105" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="H105" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I105" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="J105" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="K105" s="23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B106" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B106" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C106" s="23" t="s">
-        <v>37</v>
+      <c r="C106" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E106" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F106" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="G106" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F106" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G106" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="H106" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I106" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="J106" s="23" t="s">
-        <v>37</v>
+        <v>166</v>
+      </c>
+      <c r="I106" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J106" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="K106" s="16" t="s">
-        <v>35</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F107" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G107" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K107" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B108" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E108" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F108" s="23" t="s">
         <v>168</v>
+      </c>
+      <c r="G108" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H108" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I108" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J108" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K108" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>